<commit_message>
Update vital extraction queries and pre processing.
</commit_message>
<xml_diff>
--- a/Detection model (logistic regression)/Inzidenz_Impfstatus.xlsx
+++ b/Detection model (logistic regression)/Inzidenz_Impfstatus.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="20382"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7890B5-A545-4B3F-8AC4-470A39B32F12}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90BA5841-261D-434E-AABD-1582991358D5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{63C067C1-D90F-452D-82A9-AC3C00DC17F7}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" activeTab="1" xr2:uid="{63C067C1-D90F-452D-82A9-AC3C00DC17F7}"/>
   </bookViews>
   <sheets>
     <sheet name="Erläuterungen" sheetId="3" r:id="rId1"/>
@@ -104,7 +104,7 @@
     <t>Mit Auffrischimpfung 12-17 Jahre</t>
   </si>
   <si>
-    <t>Stand: 22.02.2022</t>
+    <t>Stand: 05.04.2022</t>
   </si>
 </sst>
 </file>
@@ -577,7 +577,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AAEA0CA-A4F5-4D63-9914-A568C3C4907C}">
   <dimension ref="A1:W17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
@@ -895,8 +895,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BB931DC8-B4B3-4A17-92B9-39B85A500E87}">
   <dimension ref="A1:AD165"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -996,19 +996,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="6">
-        <v>15.576494216918945</v>
+        <v>15.579489707946777</v>
       </c>
       <c r="G5" s="6">
-        <v>4.5371913909912109</v>
+        <v>4.5434503555297852</v>
       </c>
       <c r="H5" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="6">
-        <v>3.6509354114532471</v>
+        <v>3.6515777111053467</v>
       </c>
       <c r="J5" s="6">
-        <v>0.76013600826263428</v>
+        <v>0.76011365652084351</v>
       </c>
       <c r="K5" s="9" t="s">
         <v>11</v>
@@ -1050,19 +1050,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="6">
-        <v>23.840864181518555</v>
+        <v>23.851596832275391</v>
       </c>
       <c r="G6" s="6">
-        <v>5.9396252632141113</v>
+        <v>5.9510030746459961</v>
       </c>
       <c r="H6" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="6">
-        <v>5.1083822250366211</v>
+        <v>5.1093335151672363</v>
       </c>
       <c r="J6" s="6">
-        <v>0.91306382417678833</v>
+        <v>0.91942328214645386</v>
       </c>
       <c r="K6" s="9" t="s">
         <v>11</v>
@@ -1104,19 +1104,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="6">
-        <v>31.119380950927734</v>
+        <v>31.114517211914063</v>
       </c>
       <c r="G7" s="6">
-        <v>6.8021163940429688</v>
+        <v>6.8123188018798828</v>
       </c>
       <c r="H7" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="6">
-        <v>8.1130475997924805</v>
+        <v>8.1146059036254883</v>
       </c>
       <c r="J7" s="6">
-        <v>1.6926816701889038</v>
+        <v>1.698573112487793</v>
       </c>
       <c r="K7" s="9" t="s">
         <v>11</v>
@@ -1158,19 +1158,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="6">
-        <v>42.047256469726563</v>
+        <v>42.093276977539063</v>
       </c>
       <c r="G8" s="6">
-        <v>8.7251815795898438</v>
+        <v>8.75341796875</v>
       </c>
       <c r="H8" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="6">
-        <v>9.5820074081420898</v>
+        <v>9.5838947296142578</v>
       </c>
       <c r="J8" s="6">
-        <v>1.9930465221405029</v>
+        <v>1.9929900169372559</v>
       </c>
       <c r="K8" s="9" t="s">
         <v>11</v>
@@ -1203,28 +1203,28 @@
         <v>32</v>
       </c>
       <c r="C9" s="10">
-        <v>58.798442840576172</v>
+        <v>58.885654449462891</v>
       </c>
       <c r="D9" s="10">
-        <v>6.951685905456543</v>
+        <v>6.9515504837036133</v>
       </c>
       <c r="E9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F9" s="6">
-        <v>68.055503845214844</v>
+        <v>68.1337890625</v>
       </c>
       <c r="G9" s="6">
-        <v>12.845108985900879</v>
+        <v>12.874956130981445</v>
       </c>
       <c r="H9" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="6">
-        <v>15.436763763427734</v>
+        <v>15.466824531555176</v>
       </c>
       <c r="J9" s="6">
-        <v>3.4175972938537598</v>
+        <v>3.4228982925415039</v>
       </c>
       <c r="K9" s="9" t="s">
         <v>11</v>
@@ -1257,28 +1257,28 @@
         <v>33</v>
       </c>
       <c r="C10" s="10">
-        <v>109.45140838623047</v>
+        <v>109.71903991699219</v>
       </c>
       <c r="D10" s="10">
-        <v>12.297124862670898</v>
+        <v>12.516441345214844</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="6">
-        <v>101.14451599121094</v>
+        <v>101.25288391113281</v>
       </c>
       <c r="G10" s="6">
-        <v>17.263278961181641</v>
+        <v>17.367820739746094</v>
       </c>
       <c r="H10" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="6">
-        <v>20.638774871826172</v>
+        <v>20.67054557800293</v>
       </c>
       <c r="J10" s="6">
-        <v>4.208702564239502</v>
+        <v>4.2085738182067871</v>
       </c>
       <c r="K10" s="9" t="s">
         <v>11</v>
@@ -1311,28 +1311,28 @@
         <v>34</v>
       </c>
       <c r="C11" s="10">
-        <v>139.85098266601563</v>
+        <v>139.97805786132813</v>
       </c>
       <c r="D11" s="10">
-        <v>10.228825569152832</v>
+        <v>10.22846508026123</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="6">
-        <v>131.28704833984375</v>
+        <v>131.39395141601563</v>
       </c>
       <c r="G11" s="6">
-        <v>21.672811508178711</v>
+        <v>21.720512390136719</v>
       </c>
       <c r="H11" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="6">
-        <v>31.034753799438477</v>
+        <v>31.069412231445313</v>
       </c>
       <c r="J11" s="6">
-        <v>6.2390594482421875</v>
+        <v>6.249213695526123</v>
       </c>
       <c r="K11" s="9" t="s">
         <v>11</v>
@@ -1365,28 +1365,28 @@
         <v>35</v>
       </c>
       <c r="C12" s="10">
-        <v>167.27206420898438</v>
+        <v>167.66690063476563</v>
       </c>
       <c r="D12" s="10">
-        <v>11.18159294128418</v>
+        <v>11.181144714355469</v>
       </c>
       <c r="E12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F12" s="6">
-        <v>135.95277404785156</v>
+        <v>136.13938903808594</v>
       </c>
       <c r="G12" s="6">
-        <v>24.002128601074219</v>
+        <v>24.068347930908203</v>
       </c>
       <c r="H12" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="6">
-        <v>37.564346313476563</v>
+        <v>37.572620391845703</v>
       </c>
       <c r="J12" s="6">
-        <v>8.1979351043701172</v>
+        <v>8.2231855392456055</v>
       </c>
       <c r="K12" s="9" t="s">
         <v>11</v>
@@ -1419,28 +1419,28 @@
         <v>36</v>
       </c>
       <c r="C13" s="10">
-        <v>158.04425048828125</v>
+        <v>158.73031616210938</v>
       </c>
       <c r="D13" s="10">
-        <v>11.11857795715332</v>
+        <v>11.118156433105469</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="6">
-        <v>130.642578125</v>
+        <v>130.972900390625</v>
       </c>
       <c r="G13" s="6">
-        <v>25.131423950195313</v>
+        <v>25.222780227661133</v>
       </c>
       <c r="H13" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="6">
-        <v>42.699958801269531</v>
+        <v>42.855014801025391</v>
       </c>
       <c r="J13" s="6">
-        <v>9.3961982727050781</v>
+        <v>9.4363212585449219</v>
       </c>
       <c r="K13" s="9" t="s">
         <v>11</v>
@@ -1473,28 +1473,28 @@
         <v>37</v>
       </c>
       <c r="C14" s="10">
-        <v>150.47991943359375</v>
+        <v>151.22822570800781</v>
       </c>
       <c r="D14" s="10">
-        <v>11.057888984680176</v>
+        <v>10.951155662536621</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="6">
-        <v>110.79176330566406</v>
+        <v>111.24652862548828</v>
       </c>
       <c r="G14" s="6">
-        <v>22.739990234375</v>
+        <v>22.815650939941406</v>
       </c>
       <c r="H14" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="6">
-        <v>40.711116790771484</v>
+        <v>40.95672607421875</v>
       </c>
       <c r="J14" s="6">
-        <v>9.5630569458007813</v>
+        <v>9.5979681015014648</v>
       </c>
       <c r="K14" s="9" t="s">
         <v>11</v>
@@ -1527,28 +1527,28 @@
         <v>38</v>
       </c>
       <c r="C15" s="10">
-        <v>131.36405944824219</v>
+        <v>131.73646545410156</v>
       </c>
       <c r="D15" s="10">
-        <v>8.5516700744628906</v>
+        <v>8.5513534545898438</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="6">
-        <v>94.077995300292969</v>
+        <v>94.408668518066406</v>
       </c>
       <c r="G15" s="6">
-        <v>21.532888412475586</v>
+        <v>21.620561599731445</v>
       </c>
       <c r="H15" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="6">
-        <v>36.318500518798828</v>
+        <v>36.388134002685547</v>
       </c>
       <c r="J15" s="6">
-        <v>9.5524015426635742</v>
+        <v>9.6124238967895508</v>
       </c>
       <c r="K15" s="9" t="s">
         <v>11</v>
@@ -1581,28 +1581,28 @@
         <v>39</v>
       </c>
       <c r="C16" s="10">
-        <v>145.82960510253906</v>
+        <v>146.70413208007813</v>
       </c>
       <c r="D16" s="10">
-        <v>11.105939865112305</v>
+        <v>11.105525016784668</v>
       </c>
       <c r="E16" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F16" s="6">
-        <v>98.424346923828125</v>
+        <v>98.90667724609375</v>
       </c>
       <c r="G16" s="6">
-        <v>26.808908462524414</v>
+        <v>26.884830474853516</v>
       </c>
       <c r="H16" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="6">
-        <v>38.854354858398438</v>
+        <v>38.986625671386719</v>
       </c>
       <c r="J16" s="6">
-        <v>12.868980407714844</v>
+        <v>12.918940544128418</v>
       </c>
       <c r="K16" s="9" t="s">
         <v>11</v>
@@ -1635,28 +1635,28 @@
         <v>40</v>
       </c>
       <c r="C17" s="10">
-        <v>147.08985900878906</v>
+        <v>147.560791015625</v>
       </c>
       <c r="D17" s="10">
-        <v>9.3030376434326172</v>
+        <v>9.4527034759521484</v>
       </c>
       <c r="E17" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="6">
-        <v>105.48667144775391</v>
+        <v>105.81330871582031</v>
       </c>
       <c r="G17" s="6">
-        <v>29.594842910766602</v>
+        <v>29.649946212768555</v>
       </c>
       <c r="H17" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="6">
-        <v>48.283298492431641</v>
+        <v>48.420200347900391</v>
       </c>
       <c r="J17" s="6">
-        <v>14.993562698364258</v>
+        <v>15.028476715087891</v>
       </c>
       <c r="K17" s="9" t="s">
         <v>11</v>
@@ -1689,28 +1689,28 @@
         <v>41</v>
       </c>
       <c r="C18" s="10">
-        <v>165.06884765625</v>
+        <v>165.58943176269531</v>
       </c>
       <c r="D18" s="10">
-        <v>12.79695987701416</v>
+        <v>12.863425254821777</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="6">
-        <v>119.73936462402344</v>
+        <v>120.138671875</v>
       </c>
       <c r="G18" s="6">
-        <v>35.802066802978516</v>
+        <v>36.062320709228516</v>
       </c>
       <c r="H18" s="9" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="6">
-        <v>54.350440979003906</v>
+        <v>54.553352355957031</v>
       </c>
       <c r="J18" s="6">
-        <v>17.670129776000977</v>
+        <v>17.811700820922852</v>
       </c>
       <c r="K18" s="9" t="s">
         <v>11</v>
@@ -1742,31 +1742,31 @@
         <v>42</v>
       </c>
       <c r="C19" s="10">
-        <v>227.309326171875</v>
+        <v>228.16297912597656</v>
       </c>
       <c r="D19" s="10">
-        <v>17.423860549926758</v>
+        <v>17.674701690673828</v>
       </c>
       <c r="E19" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="6">
-        <v>176.191162109375</v>
+        <v>177.06596374511719</v>
       </c>
       <c r="G19" s="6">
-        <v>56.713817596435547</v>
+        <v>57.142707824707031</v>
       </c>
       <c r="H19" s="6">
-        <v>28.15020751953125</v>
+        <v>29.9613037109375</v>
       </c>
       <c r="I19" s="6">
-        <v>86.241897583007813</v>
+        <v>86.675483703613281</v>
       </c>
       <c r="J19" s="6">
-        <v>31.046981811523438</v>
+        <v>31.245054244995117</v>
       </c>
       <c r="K19" s="6">
-        <v>11.37730598449707</v>
+        <v>11.505082130432129</v>
       </c>
       <c r="L19" s="13"/>
       <c r="M19" s="13"/>
@@ -1795,31 +1795,31 @@
         <v>43</v>
       </c>
       <c r="C20" s="10">
-        <v>317.04446411132813</v>
+        <v>319.3800048828125</v>
       </c>
       <c r="D20" s="10">
-        <v>27.354639053344727</v>
+        <v>27.951986312866211</v>
       </c>
       <c r="E20" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="6">
-        <v>226.83853149414063</v>
+        <v>228.24722290039063</v>
       </c>
       <c r="G20" s="6">
-        <v>76.701698303222656</v>
+        <v>77.39703369140625</v>
       </c>
       <c r="H20" s="6">
-        <v>43.242805480957031</v>
+        <v>44.699871063232422</v>
       </c>
       <c r="I20" s="6">
-        <v>111.70655822753906</v>
+        <v>112.49837493896484</v>
       </c>
       <c r="J20" s="6">
-        <v>46.482967376708984</v>
+        <v>46.892833709716797</v>
       </c>
       <c r="K20" s="6">
-        <v>13.400918006896973</v>
+        <v>13.502330780029297</v>
       </c>
       <c r="L20" s="13"/>
       <c r="M20" s="13"/>
@@ -1848,31 +1848,31 @@
         <v>44</v>
       </c>
       <c r="C21" s="10">
-        <v>337.24786376953125</v>
+        <v>340.99136352539063</v>
       </c>
       <c r="D21" s="10">
-        <v>29.116680145263672</v>
+        <v>29.689472198486328</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="6">
-        <v>265.99908447265625</v>
+        <v>268.38327026367188</v>
       </c>
       <c r="G21" s="6">
-        <v>94.031585693359375</v>
+        <v>95.132537841796875</v>
       </c>
       <c r="H21" s="6">
-        <v>42.874034881591797</v>
+        <v>44.969005584716797</v>
       </c>
       <c r="I21" s="6">
-        <v>143.69314575195313</v>
+        <v>144.75904846191406</v>
       </c>
       <c r="J21" s="6">
-        <v>58.868053436279297</v>
+        <v>59.462909698486328</v>
       </c>
       <c r="K21" s="6">
-        <v>16.573247909545898</v>
+        <v>16.821010589599609</v>
       </c>
       <c r="L21" s="13"/>
       <c r="M21" s="13"/>
@@ -1901,31 +1901,31 @@
         <v>45</v>
       </c>
       <c r="C22" s="10">
-        <v>489.00570678710938</v>
+        <v>494.7481689453125</v>
       </c>
       <c r="D22" s="10">
-        <v>50.63336181640625</v>
+        <v>51.461414337158203</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="6">
-        <v>326.10321044921875</v>
+        <v>329.8192138671875</v>
       </c>
       <c r="G22" s="6">
-        <v>119.03044128417969</v>
+        <v>120.78118896484375</v>
       </c>
       <c r="H22" s="6">
-        <v>56.454917907714844</v>
+        <v>59.339778900146484</v>
       </c>
       <c r="I22" s="6">
-        <v>180.66596984863281</v>
+        <v>182.39974975585938</v>
       </c>
       <c r="J22" s="6">
-        <v>75.64752197265625</v>
+        <v>76.635581970214844</v>
       </c>
       <c r="K22" s="6">
-        <v>17.662551879882813</v>
+        <v>17.98570442199707</v>
       </c>
       <c r="L22" s="13"/>
       <c r="M22" s="13"/>
@@ -1954,31 +1954,31 @@
         <v>46</v>
       </c>
       <c r="C23" s="10">
-        <v>530.22906494140625</v>
+        <v>541.16571044921875</v>
       </c>
       <c r="D23" s="10">
-        <v>54.414314270019531</v>
+        <v>55.644096374511719</v>
       </c>
       <c r="E23" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="6">
-        <v>352.58892822265625</v>
+        <v>359.59881591796875</v>
       </c>
       <c r="G23" s="6">
-        <v>140.13398742675781</v>
+        <v>144.43963623046875</v>
       </c>
       <c r="H23" s="6">
-        <v>59.637115478515625</v>
+        <v>63.652507781982422</v>
       </c>
       <c r="I23" s="6">
-        <v>192.56968688964844</v>
+        <v>195.91624450683594</v>
       </c>
       <c r="J23" s="6">
-        <v>86.281143188476563</v>
+        <v>88.068359375</v>
       </c>
       <c r="K23" s="6">
-        <v>21.950143814086914</v>
+        <v>22.574935913085938</v>
       </c>
       <c r="L23" s="13"/>
       <c r="M23" s="13"/>
@@ -2007,31 +2007,31 @@
         <v>47</v>
       </c>
       <c r="C24" s="10">
-        <v>534.20196533203125</v>
+        <v>548.7945556640625</v>
       </c>
       <c r="D24" s="10">
-        <v>58.123565673828125</v>
+        <v>59.686405181884766</v>
       </c>
       <c r="E24" s="9" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="6">
-        <v>374.02935791015625</v>
+        <v>384.30523681640625</v>
       </c>
       <c r="G24" s="6">
-        <v>139.32038879394531</v>
+        <v>143.8603515625</v>
       </c>
       <c r="H24" s="6">
-        <v>61.134578704833984</v>
+        <v>64.302833557128906</v>
       </c>
       <c r="I24" s="6">
-        <v>215.01756286621094</v>
+        <v>221.16719055175781</v>
       </c>
       <c r="J24" s="6">
-        <v>86.374763488769531</v>
+        <v>89.060745239257813</v>
       </c>
       <c r="K24" s="6">
-        <v>24.510993957519531</v>
+        <v>25.033468246459961</v>
       </c>
       <c r="L24" s="13"/>
       <c r="M24" s="13"/>
@@ -2060,31 +2060,31 @@
         <v>48</v>
       </c>
       <c r="C25" s="10">
-        <v>500.47964477539063</v>
+        <v>511.35379028320313</v>
       </c>
       <c r="D25" s="10">
-        <v>56.311492919921875</v>
+        <v>57.741035461425781</v>
       </c>
       <c r="E25" s="10">
-        <v>19.962072372436523</v>
+        <v>19.978689193725586</v>
       </c>
       <c r="F25" s="6">
-        <v>343.64126586914063</v>
+        <v>349.98968505859375</v>
       </c>
       <c r="G25" s="6">
-        <v>125.86140441894531</v>
+        <v>129.84626770019531</v>
       </c>
       <c r="H25" s="6">
-        <v>47.501602172851563</v>
+        <v>49.186248779296875</v>
       </c>
       <c r="I25" s="6">
-        <v>208.05210876464844</v>
+        <v>211.4039306640625</v>
       </c>
       <c r="J25" s="6">
-        <v>73.430519104003906</v>
+        <v>75.151405334472656</v>
       </c>
       <c r="K25" s="6">
-        <v>19.919050216674805</v>
+        <v>20.451757431030273</v>
       </c>
       <c r="L25" s="13"/>
       <c r="M25" s="13"/>
@@ -2113,31 +2113,31 @@
         <v>49</v>
       </c>
       <c r="C26" s="10">
-        <v>449.0440673828125</v>
+        <v>458.69580078125</v>
       </c>
       <c r="D26" s="10">
-        <v>54.054981231689453</v>
+        <v>55.060882568359375</v>
       </c>
       <c r="E26" s="10">
-        <v>14.23892879486084</v>
+        <v>18.315391540527344</v>
       </c>
       <c r="F26" s="6">
-        <v>298.07894897460938</v>
+        <v>305.02093505859375</v>
       </c>
       <c r="G26" s="6">
-        <v>109.15361022949219</v>
+        <v>112.61207580566406</v>
       </c>
       <c r="H26" s="6">
-        <v>37.717304229736328</v>
+        <v>39.174015045166016</v>
       </c>
       <c r="I26" s="6">
-        <v>192.92941284179688</v>
+        <v>195.61248779296875</v>
       </c>
       <c r="J26" s="6">
-        <v>63.716941833496094</v>
+        <v>65.246223449707031</v>
       </c>
       <c r="K26" s="6">
-        <v>15.659321784973145</v>
+        <v>16.007625579833984</v>
       </c>
       <c r="L26" s="13"/>
       <c r="M26" s="13"/>
@@ -2166,31 +2166,31 @@
         <v>50</v>
       </c>
       <c r="C27" s="10">
-        <v>369.33050537109375</v>
+        <v>378.64093017578125</v>
       </c>
       <c r="D27" s="10">
-        <v>48.585296630859375</v>
+        <v>49.932506561279297</v>
       </c>
       <c r="E27" s="10">
-        <v>10.903539657592773</v>
+        <v>10.906182289123535</v>
       </c>
       <c r="F27" s="6">
-        <v>245.50021362304688</v>
+        <v>252.13395690917969</v>
       </c>
       <c r="G27" s="6">
-        <v>93.096115112304688</v>
+        <v>96.065528869628906</v>
       </c>
       <c r="H27" s="6">
-        <v>28.43560791015625</v>
+        <v>29.440858840942383</v>
       </c>
       <c r="I27" s="6">
-        <v>156.40425109863281</v>
+        <v>160.36473083496094</v>
       </c>
       <c r="J27" s="6">
-        <v>48.593505859375</v>
+        <v>49.858909606933594</v>
       </c>
       <c r="K27" s="6">
-        <v>10.915305137634277</v>
+        <v>11.177370071411133</v>
       </c>
     </row>
     <row r="28" spans="1:30" x14ac:dyDescent="0.25">
@@ -2201,31 +2201,31 @@
         <v>51</v>
       </c>
       <c r="C28" s="10">
-        <v>233.52191162109375</v>
+        <v>237.64480590820313</v>
       </c>
       <c r="D28" s="10">
-        <v>44.592723846435547</v>
+        <v>46.775962829589844</v>
       </c>
       <c r="E28" s="10">
-        <v>9.5820627212524414</v>
+        <v>10.381396293640137</v>
       </c>
       <c r="F28" s="6">
-        <v>166.38655090332031</v>
+        <v>170.08798217773438</v>
       </c>
       <c r="G28" s="6">
-        <v>76.944992065429688</v>
+        <v>79.344261169433594</v>
       </c>
       <c r="H28" s="6">
-        <v>27.638254165649414</v>
+        <v>28.509872436523438</v>
       </c>
       <c r="I28" s="6">
-        <v>111.44602966308594</v>
+        <v>113.55418395996094</v>
       </c>
       <c r="J28" s="6">
-        <v>35.455322265625</v>
+        <v>36.187126159667969</v>
       </c>
       <c r="K28" s="6">
-        <v>9.3496131896972656</v>
+        <v>9.4942455291748047</v>
       </c>
     </row>
     <row r="29" spans="1:30" x14ac:dyDescent="0.25">
@@ -2236,31 +2236,31 @@
         <v>52</v>
       </c>
       <c r="C29" s="10">
-        <v>208.93344116210938</v>
+        <v>214.46693420410156</v>
       </c>
       <c r="D29" s="10">
-        <v>69.608558654785156</v>
+        <v>72.118942260742188</v>
       </c>
       <c r="E29" s="10">
-        <v>23.862415313720703</v>
+        <v>24.428625106811523</v>
       </c>
       <c r="F29" s="6">
-        <v>171.08482360839844</v>
+        <v>175.22637939453125</v>
       </c>
       <c r="G29" s="6">
-        <v>110.59500885009766</v>
+        <v>114.44139862060547</v>
       </c>
       <c r="H29" s="6">
-        <v>46.008129119873047</v>
+        <v>47.393321990966797</v>
       </c>
       <c r="I29" s="6">
-        <v>108.58554077148438</v>
+        <v>110.95841217041016</v>
       </c>
       <c r="J29" s="6">
-        <v>41.610507965087891</v>
+        <v>42.623996734619141</v>
       </c>
       <c r="K29" s="6">
-        <v>15.711198806762695</v>
+        <v>16.151958465576172</v>
       </c>
     </row>
     <row r="30" spans="1:30" x14ac:dyDescent="0.25">
@@ -2271,31 +2271,31 @@
         <v>1</v>
       </c>
       <c r="C30" s="10">
-        <v>271.660400390625</v>
+        <v>279.9549560546875</v>
       </c>
       <c r="D30" s="10">
-        <v>147.65374755859375</v>
+        <v>153.20974731445313</v>
       </c>
       <c r="E30" s="10">
-        <v>70.409126281738281</v>
+        <v>72.157737731933594</v>
       </c>
       <c r="F30" s="6">
-        <v>189.6063232421875</v>
+        <v>196.48655700683594</v>
       </c>
       <c r="G30" s="6">
-        <v>180.69644165039063</v>
+        <v>187.83407592773438</v>
       </c>
       <c r="H30" s="6">
-        <v>89.775276184082031</v>
+        <v>92.132102966308594</v>
       </c>
       <c r="I30" s="6">
-        <v>106.08270263671875</v>
+        <v>108.50118255615234</v>
       </c>
       <c r="J30" s="6">
-        <v>54.091651916503906</v>
+        <v>55.630519866943359</v>
       </c>
       <c r="K30" s="6">
-        <v>22.148981094360352</v>
+        <v>22.658170700073242</v>
       </c>
     </row>
     <row r="31" spans="1:30" x14ac:dyDescent="0.25">
@@ -2306,31 +2306,31 @@
         <v>2</v>
       </c>
       <c r="C31" s="10">
-        <v>339.59783935546875</v>
+        <v>354.50820922851563</v>
       </c>
       <c r="D31" s="10">
-        <v>208.03167724609375</v>
+        <v>215.03427124023438</v>
       </c>
       <c r="E31" s="10">
-        <v>95.881790161132813</v>
+        <v>97.163429260253906</v>
       </c>
       <c r="F31" s="6">
-        <v>178.86332702636719</v>
+        <v>187.15966796875</v>
       </c>
       <c r="G31" s="6">
-        <v>180.84390258789063</v>
+        <v>190.16102600097656</v>
       </c>
       <c r="H31" s="6">
-        <v>92.619392395019531</v>
+        <v>96.412445068359375</v>
       </c>
       <c r="I31" s="6">
-        <v>75.2789306640625</v>
+        <v>77.617240905761719</v>
       </c>
       <c r="J31" s="6">
-        <v>45.791896820068359</v>
+        <v>47.613735198974609</v>
       </c>
       <c r="K31" s="6">
-        <v>22.239755630493164</v>
+        <v>23.064493179321289</v>
       </c>
     </row>
     <row r="32" spans="1:30" x14ac:dyDescent="0.25">
@@ -2341,31 +2341,31 @@
         <v>3</v>
       </c>
       <c r="C32" s="10">
-        <v>429.80499267578125</v>
+        <v>450.94583129882813</v>
       </c>
       <c r="D32" s="10">
-        <v>219.05317687988281</v>
+        <v>235.06661987304688</v>
       </c>
       <c r="E32" s="10">
-        <v>75.137176513671875</v>
+        <v>80.451744079589844</v>
       </c>
       <c r="F32" s="6">
-        <v>217.02748107910156</v>
+        <v>225.69975280761719</v>
       </c>
       <c r="G32" s="6">
-        <v>193.66456604003906</v>
+        <v>209.570556640625</v>
       </c>
       <c r="H32" s="6">
-        <v>105.96909332275391</v>
+        <v>112.92941284179688</v>
       </c>
       <c r="I32" s="6">
-        <v>79.818901062011719</v>
+        <v>82.221992492675781</v>
       </c>
       <c r="J32" s="6">
-        <v>49.134490966796875</v>
+        <v>53.509426116943359</v>
       </c>
       <c r="K32" s="6">
-        <v>25.362758636474609</v>
+        <v>26.945652008056641</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -2376,31 +2376,31 @@
         <v>4</v>
       </c>
       <c r="C33" s="10">
-        <v>494.81582641601563</v>
+        <v>540.42767333984375</v>
       </c>
       <c r="D33" s="10">
-        <v>226.16311645507813</v>
+        <v>255.98609924316406</v>
       </c>
       <c r="E33" s="10">
-        <v>77.244010925292969</v>
+        <v>86.779647827148438</v>
       </c>
       <c r="F33" s="6">
-        <v>236.28059387207031</v>
+        <v>255.21260070800781</v>
       </c>
       <c r="G33" s="6">
-        <v>185.927490234375</v>
+        <v>211.75428771972656</v>
       </c>
       <c r="H33" s="6">
-        <v>106.06025695800781</v>
+        <v>118.46305084228516</v>
       </c>
       <c r="I33" s="6">
-        <v>84.781517028808594</v>
+        <v>90.665985107421875</v>
       </c>
       <c r="J33" s="6">
-        <v>47.586643218994141</v>
+        <v>54.088367462158203</v>
       </c>
       <c r="K33" s="6">
-        <v>26.328332901000977</v>
+        <v>29.253576278686523</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -2411,31 +2411,31 @@
         <v>5</v>
       </c>
       <c r="C34" s="10">
-        <v>491.05706787109375</v>
+        <v>547.45452880859375</v>
       </c>
       <c r="D34" s="10">
-        <v>225.92449951171875</v>
+        <v>256.13449096679688</v>
       </c>
       <c r="E34" s="10">
-        <v>71.192543029785156</v>
+        <v>81.130302429199219</v>
       </c>
       <c r="F34" s="6">
-        <v>247.02659606933594</v>
+        <v>269.998291015625</v>
       </c>
       <c r="G34" s="6">
-        <v>184.80574035644531</v>
+        <v>211.25323486328125</v>
       </c>
       <c r="H34" s="6">
-        <v>108.47478485107422</v>
+        <v>122.54711151123047</v>
       </c>
       <c r="I34" s="6">
-        <v>101.89260101318359</v>
+        <v>111.28116607666016</v>
       </c>
       <c r="J34" s="6">
-        <v>48.419353485107422</v>
+        <v>56.525466918945313</v>
       </c>
       <c r="K34" s="6">
-        <v>28.346929550170898</v>
+        <v>32.386493682861328</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -2446,98 +2446,242 @@
         <v>6</v>
       </c>
       <c r="C35" s="6">
-        <v>425.70223999023438</v>
+        <v>490.5758056640625</v>
       </c>
       <c r="D35" s="6">
-        <v>223.49433898925781</v>
+        <v>263.06201171875</v>
       </c>
       <c r="E35" s="6">
-        <v>82.767501831054688</v>
+        <v>95.418014526367188</v>
       </c>
       <c r="F35" s="6">
-        <v>224.56382751464844</v>
+        <v>259.24334716796875</v>
       </c>
       <c r="G35" s="6">
-        <v>191.15243530273438</v>
+        <v>227.93902587890625</v>
       </c>
       <c r="H35" s="6">
-        <v>118.05306243896484</v>
+        <v>141.06892395019531</v>
       </c>
       <c r="I35" s="6">
-        <v>97.123367309570313</v>
+        <v>113.61431884765625</v>
       </c>
       <c r="J35" s="6">
-        <v>56.632122039794922</v>
+        <v>65.874710083007813</v>
       </c>
       <c r="K35" s="6">
-        <v>33.151020050048828</v>
+        <v>40.134658813476563</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="A36" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B36" s="2">
+        <v>7</v>
+      </c>
+      <c r="C36" s="6">
+        <v>365.7757568359375</v>
+      </c>
+      <c r="D36" s="6">
+        <v>232.00617980957031</v>
+      </c>
+      <c r="E36" s="6">
+        <v>99.559761047363281</v>
+      </c>
+      <c r="F36" s="6">
+        <v>225.4832763671875</v>
+      </c>
+      <c r="G36" s="6">
+        <v>206.24375915527344</v>
+      </c>
+      <c r="H36" s="6">
+        <v>140.08016967773438</v>
+      </c>
+      <c r="I36" s="6">
+        <v>102.29685974121094</v>
+      </c>
+      <c r="J36" s="6">
+        <v>66.625686645507813</v>
+      </c>
+      <c r="K36" s="6">
+        <v>43.00048828125</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="A37" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B37" s="2">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6">
+        <v>311.01739501953125</v>
+      </c>
+      <c r="D37" s="6">
+        <v>195.32931518554688</v>
+      </c>
+      <c r="E37" s="6">
+        <v>108.71251678466797</v>
+      </c>
+      <c r="F37" s="6">
+        <v>202.10893249511719</v>
+      </c>
+      <c r="G37" s="6">
+        <v>175.56805419921875</v>
+      </c>
+      <c r="H37" s="6">
+        <v>135.97560119628906</v>
+      </c>
+      <c r="I37" s="6">
+        <v>97.59765625</v>
+      </c>
+      <c r="J37" s="6">
+        <v>61.440284729003906</v>
+      </c>
+      <c r="K37" s="6">
+        <v>44.062320709228516</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
+      <c r="A38" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B38" s="2">
+        <v>9</v>
+      </c>
+      <c r="C38" s="6">
+        <v>274.38662719726563</v>
+      </c>
+      <c r="D38" s="6">
+        <v>187.81086730957031</v>
+      </c>
+      <c r="E38" s="6">
+        <v>133.20758056640625</v>
+      </c>
+      <c r="F38" s="6">
+        <v>171.49378967285156</v>
+      </c>
+      <c r="G38" s="6">
+        <v>176.67901611328125</v>
+      </c>
+      <c r="H38" s="6">
+        <v>157.38577270507813</v>
+      </c>
+      <c r="I38" s="6">
+        <v>87.752182006835938</v>
+      </c>
+      <c r="J38" s="6">
+        <v>61.103157043457031</v>
+      </c>
+      <c r="K38" s="6">
+        <v>45.558021545410156</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="A39" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B39" s="2">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6">
+        <v>273.8135986328125</v>
+      </c>
+      <c r="D39" s="6">
+        <v>214.14093017578125</v>
+      </c>
+      <c r="E39" s="6">
+        <v>167.59466552734375</v>
+      </c>
+      <c r="F39" s="6">
+        <v>169.29322814941406</v>
+      </c>
+      <c r="G39" s="6">
+        <v>181.11723327636719</v>
+      </c>
+      <c r="H39" s="6">
+        <v>172.02052307128906</v>
+      </c>
+      <c r="I39" s="6">
+        <v>89.202407836914063</v>
+      </c>
+      <c r="J39" s="6">
+        <v>58.501285552978516</v>
+      </c>
+      <c r="K39" s="6">
+        <v>51.736564636230469</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
+      <c r="A40" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B40" s="2">
+        <v>11</v>
+      </c>
+      <c r="C40" s="6">
+        <v>243.9395751953125</v>
+      </c>
+      <c r="D40" s="6">
+        <v>181.45491027832031</v>
+      </c>
+      <c r="E40" s="6">
+        <v>134.27107238769531</v>
+      </c>
+      <c r="F40" s="6">
+        <v>140.27223205566406</v>
+      </c>
+      <c r="G40" s="6">
+        <v>156.82878112792969</v>
+      </c>
+      <c r="H40" s="6">
+        <v>155.20498657226563</v>
+      </c>
+      <c r="I40" s="6">
+        <v>81.214103698730469</v>
+      </c>
+      <c r="J40" s="6">
+        <v>56.381351470947266</v>
+      </c>
+      <c r="K40" s="6">
+        <v>52.724033355712891</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="A41" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B41" s="2">
+        <v>12</v>
+      </c>
+      <c r="C41" s="6">
+        <v>202.58697509765625</v>
+      </c>
+      <c r="D41" s="6">
+        <v>142.62942504882813</v>
+      </c>
+      <c r="E41" s="6">
+        <v>115.64024353027344</v>
+      </c>
+      <c r="F41" s="6">
+        <v>141.96604919433594</v>
+      </c>
+      <c r="G41" s="6">
+        <v>122.65164184570313</v>
+      </c>
+      <c r="H41" s="6">
+        <v>131.66410827636719</v>
+      </c>
+      <c r="I41" s="6">
+        <v>100.51689910888672</v>
+      </c>
+      <c r="J41" s="6">
+        <v>52.169082641601563</v>
+      </c>
+      <c r="K41" s="6">
+        <v>47.485225677490234</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C42" s="6"/>
@@ -3913,8 +4057,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A52C268F-58D3-4BD0-95F5-EC5AFA40F9F0}">
   <dimension ref="A1:BP368"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A37" sqref="A37"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3986,19 +4130,19 @@
         <v>11</v>
       </c>
       <c r="F5" s="5">
-        <v>0.89633160829544067</v>
+        <v>0.8965039849281311</v>
       </c>
       <c r="G5" s="27">
-        <v>0.11734115332365036</v>
+        <v>0.11733444035053253</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I5" s="5">
-        <v>1.1516373157501221</v>
+        <v>1.1518399715423584</v>
       </c>
       <c r="J5" s="5">
-        <v>0.27392289042472839</v>
+        <v>0.27391484379768372</v>
       </c>
       <c r="K5" s="7" t="s">
         <v>11</v>
@@ -4077,19 +4221,19 @@
         <v>11</v>
       </c>
       <c r="F6" s="5">
-        <v>1.3517427444458008</v>
+        <v>1.3520278930664063</v>
       </c>
       <c r="G6" s="27">
-        <v>0.10522958636283875</v>
+        <v>0.10522402077913284</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I6" s="5">
-        <v>1.7702314853668213</v>
+        <v>1.7705610990524292</v>
       </c>
       <c r="J6" s="5">
-        <v>0.32563814520835876</v>
+        <v>0.32562908530235291</v>
       </c>
       <c r="K6" s="7" t="s">
         <v>11</v>
@@ -4168,19 +4312,19 @@
         <v>11</v>
       </c>
       <c r="F7" s="5">
-        <v>1.842323899269104</v>
+        <v>1.8427330255508423</v>
       </c>
       <c r="G7" s="27">
-        <v>0.1849837452173233</v>
+        <v>0.18497374653816223</v>
       </c>
       <c r="H7" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I7" s="5">
-        <v>2.903071403503418</v>
+        <v>2.9036290645599365</v>
       </c>
       <c r="J7" s="5">
-        <v>0.43356409668922424</v>
+        <v>0.43355187773704529</v>
       </c>
       <c r="K7" s="7" t="s">
         <v>11</v>
@@ -4259,19 +4403,19 @@
         <v>11</v>
       </c>
       <c r="F8" s="5">
-        <v>2.5708653926849365</v>
+        <v>2.5714592933654785</v>
       </c>
       <c r="G8" s="27">
-        <v>0.2633836567401886</v>
+        <v>0.26815721392631531</v>
       </c>
       <c r="H8" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I8" s="5">
-        <v>3.7586879730224609</v>
+        <v>3.7594282627105713</v>
       </c>
       <c r="J8" s="5">
-        <v>0.49128317832946777</v>
+        <v>0.49126926064491272</v>
       </c>
       <c r="K8" s="7" t="s">
         <v>11</v>
@@ -4341,7 +4485,7 @@
         <v>32</v>
       </c>
       <c r="C9" s="5">
-        <v>0.91782933473587036</v>
+        <v>0.91784751415252686</v>
       </c>
       <c r="D9" s="5">
         <v>0</v>
@@ -4350,19 +4494,19 @@
         <v>11</v>
       </c>
       <c r="F9" s="5">
-        <v>4.5622072219848633</v>
+        <v>4.5818796157836914</v>
       </c>
       <c r="G9" s="27">
-        <v>0.30280578136444092</v>
+        <v>0.3071734607219696</v>
       </c>
       <c r="H9" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I9" s="5">
-        <v>5.576632022857666</v>
+        <v>5.5777573585510254</v>
       </c>
       <c r="J9" s="5">
-        <v>0.89225244522094727</v>
+        <v>0.89222466945648193</v>
       </c>
       <c r="K9" s="7" t="s">
         <v>11</v>
@@ -4432,28 +4576,28 @@
         <v>33</v>
       </c>
       <c r="C10" s="5">
-        <v>1.5033724308013916</v>
+        <v>1.5034043788909912</v>
       </c>
       <c r="D10" s="5">
-        <v>0.21959151327610016</v>
+        <v>0.21958670020103455</v>
       </c>
       <c r="E10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F10" s="5">
-        <v>6.6529879570007324</v>
+        <v>6.6674065589904785</v>
       </c>
       <c r="G10" s="27">
-        <v>0.4719633162021637</v>
+        <v>0.47192955017089844</v>
       </c>
       <c r="H10" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I10" s="5">
-        <v>8.1071081161499023</v>
+        <v>8.1362781524658203</v>
       </c>
       <c r="J10" s="5">
-        <v>1.1641092300415039</v>
+        <v>1.1640735864639282</v>
       </c>
       <c r="K10" s="7" t="s">
         <v>11</v>
@@ -4523,28 +4667,28 @@
         <v>34</v>
       </c>
       <c r="C11" s="5">
-        <v>1.6064172983169556</v>
+        <v>1.6064574718475342</v>
       </c>
       <c r="D11" s="5">
-        <v>0.17635907232761383</v>
+        <v>0.1763528436422348</v>
       </c>
       <c r="E11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F11" s="5">
-        <v>9.513554573059082</v>
+        <v>9.5160694122314453</v>
       </c>
       <c r="G11" s="27">
-        <v>0.53306281566619873</v>
+        <v>0.53301870822906494</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="5">
-        <v>11.45596981048584</v>
+        <v>11.486437797546387</v>
       </c>
       <c r="J11" s="5">
-        <v>1.5882183313369751</v>
+        <v>1.5933425426483154</v>
       </c>
       <c r="K11" s="7" t="s">
         <v>11</v>
@@ -4614,7 +4758,7 @@
         <v>35</v>
       </c>
       <c r="C12" s="5">
-        <v>1.5599493980407715</v>
+        <v>1.5599944591522217</v>
       </c>
       <c r="D12" s="5">
         <v>0</v>
@@ -4623,19 +4767,19 @@
         <v>11</v>
       </c>
       <c r="F12" s="5">
-        <v>8.9025154113769531</v>
+        <v>8.9320535659790039</v>
       </c>
       <c r="G12" s="27">
-        <v>0.633339524269104</v>
+        <v>0.63688105344772339</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I12" s="5">
-        <v>13.405652046203613</v>
+        <v>13.408603668212891</v>
       </c>
       <c r="J12" s="5">
-        <v>2.025252103805542</v>
+        <v>2.0353915691375732</v>
       </c>
       <c r="K12" s="7" t="s">
         <v>11</v>
@@ -4705,28 +4849,28 @@
         <v>36</v>
       </c>
       <c r="C13" s="5">
-        <v>1.8709499835968018</v>
+        <v>1.9050359725952148</v>
       </c>
       <c r="D13" s="5">
-        <v>0.12218217551708221</v>
+        <v>0.12217754870653152</v>
       </c>
       <c r="E13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F13" s="5">
-        <v>8.0223388671875</v>
+        <v>8.0663919448852539</v>
       </c>
       <c r="G13" s="27">
-        <v>0.57952886819839478</v>
+        <v>0.57600516080856323</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I13" s="5">
-        <v>15.131960868835449</v>
+        <v>15.193523406982422</v>
       </c>
       <c r="J13" s="5">
-        <v>2.1318256855010986</v>
+        <v>2.1368114948272705</v>
       </c>
       <c r="K13" s="7" t="s">
         <v>11</v>
@@ -4796,28 +4940,28 @@
         <v>37</v>
       </c>
       <c r="C14" s="5">
-        <v>1.4479410648345947</v>
+        <v>1.5186393260955811</v>
       </c>
       <c r="D14" s="5">
-        <v>0.10632585734128952</v>
+        <v>0.10632190108299255</v>
       </c>
       <c r="E14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F14" s="5">
-        <v>6.8319687843322754</v>
+        <v>6.8768253326416016</v>
       </c>
       <c r="G14" s="27">
-        <v>0.50097030401229858</v>
+        <v>0.50769138336181641</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I14" s="5">
-        <v>13.707644462585449</v>
+        <v>13.76993465423584</v>
       </c>
       <c r="J14" s="5">
-        <v>1.9518496990203857</v>
+        <v>1.9568183422088623</v>
       </c>
       <c r="K14" s="7" t="s">
         <v>11</v>
@@ -4887,28 +5031,28 @@
         <v>38</v>
       </c>
       <c r="C15" s="5">
-        <v>1.0234261751174927</v>
+        <v>1.023479700088501</v>
       </c>
       <c r="D15" s="5">
-        <v>0.19003711640834808</v>
+        <v>0.19003006815910339</v>
       </c>
       <c r="E15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F15" s="5">
-        <v>5.6275997161865234</v>
+        <v>5.6586790084838867</v>
       </c>
       <c r="G15" s="27">
-        <v>0.54538899660110474</v>
+        <v>0.54533559083938599</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I15" s="5">
-        <v>13.081828117370605</v>
+        <v>13.115262985229492</v>
       </c>
       <c r="J15" s="5">
-        <v>2.0411972999572754</v>
+        <v>2.0461592674255371</v>
       </c>
       <c r="K15" s="7" t="s">
         <v>11</v>
@@ -4978,7 +5122,7 @@
         <v>39</v>
       </c>
       <c r="C16" s="5">
-        <v>1.1292948722839355</v>
+        <v>1.1293619871139526</v>
       </c>
       <c r="D16" s="5">
         <v>0</v>
@@ -4987,19 +5131,19 @@
         <v>11</v>
       </c>
       <c r="F16" s="5">
-        <v>5.5007767677307129</v>
+        <v>5.532562255859375</v>
       </c>
       <c r="G16" s="27">
-        <v>0.6254429817199707</v>
+        <v>0.62538093328475952</v>
       </c>
       <c r="H16" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="5">
-        <v>13.344836235046387</v>
+        <v>13.439489364624023</v>
       </c>
       <c r="J16" s="5">
-        <v>2.4790675640106201</v>
+        <v>2.4941012859344482</v>
       </c>
       <c r="K16" s="7" t="s">
         <v>11</v>
@@ -5069,28 +5213,28 @@
         <v>40</v>
       </c>
       <c r="C17" s="5">
-        <v>0.88423073291778564</v>
+        <v>0.88428819179534912</v>
       </c>
       <c r="D17" s="5">
-        <v>7.5024493038654327E-2</v>
+        <v>7.5021453201770782E-2</v>
       </c>
       <c r="E17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F17" s="5">
-        <v>5.2443552017211914</v>
+        <v>5.2614350318908691</v>
       </c>
       <c r="G17" s="27">
-        <v>0.57415610551834106</v>
+        <v>0.57409882545471191</v>
       </c>
       <c r="H17" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="5">
-        <v>15.035052299499512</v>
+        <v>15.192448616027832</v>
       </c>
       <c r="J17" s="5">
-        <v>2.9794900417327881</v>
+        <v>2.9793918132781982</v>
       </c>
       <c r="K17" s="7" t="s">
         <v>11</v>
@@ -5104,28 +5248,28 @@
         <v>41</v>
       </c>
       <c r="C18" s="5">
-        <v>1.4881651401519775</v>
+        <v>1.4882683753967285</v>
       </c>
       <c r="D18" s="5">
-        <v>6.699979305267334E-2</v>
+        <v>6.699700653553009E-2</v>
       </c>
       <c r="E18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="5">
-        <v>6.0304832458496094</v>
+        <v>6.0481534004211426</v>
       </c>
       <c r="G18" s="27">
-        <v>0.66470927000045776</v>
+        <v>0.6710008978843689</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>11</v>
       </c>
       <c r="I18" s="5">
-        <v>17.53040885925293</v>
+        <v>17.597856521606445</v>
       </c>
       <c r="J18" s="5">
-        <v>3.5086379051208496</v>
+        <v>3.5389840602874756</v>
       </c>
       <c r="K18" s="7" t="s">
         <v>11</v>
@@ -5139,31 +5283,31 @@
         <v>42</v>
       </c>
       <c r="C19" s="5">
-        <v>1.5544562339782715</v>
+        <v>1.5545696020126343</v>
       </c>
       <c r="D19" s="5">
-        <v>0.18870607018470764</v>
+        <v>0.18869787454605103</v>
       </c>
       <c r="E19" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F19" s="5">
-        <v>7.9270405769348145</v>
+        <v>7.9692573547363281</v>
       </c>
       <c r="G19" s="27">
-        <v>1.0710824728012085</v>
+        <v>1.0772727727890015</v>
       </c>
       <c r="H19" s="5">
-        <v>1.4436002969741821</v>
+        <v>1.8048977851867676</v>
       </c>
       <c r="I19" s="5">
-        <v>28.042608261108398</v>
+        <v>28.145431518554688</v>
       </c>
       <c r="J19" s="5">
-        <v>5.7191810607910156</v>
+        <v>5.7598333358764648</v>
       </c>
       <c r="K19" s="5">
-        <v>4.0907168388366699</v>
+        <v>4.090695858001709</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
@@ -5174,31 +5318,31 @@
         <v>43</v>
       </c>
       <c r="C20" s="5">
-        <v>1.9865957498550415</v>
+        <v>1.9867488145828247</v>
       </c>
       <c r="D20" s="5">
-        <v>0.23942790925502777</v>
+        <v>0.23941744863986969</v>
       </c>
       <c r="E20" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F20" s="5">
-        <v>9.3738203048706055</v>
+        <v>9.448969841003418</v>
       </c>
       <c r="G20" s="27">
-        <v>1.2658077478408813</v>
+        <v>1.2750540971755981</v>
       </c>
       <c r="H20" s="5">
-        <v>2.031541109085083</v>
+        <v>2.0318124294281006</v>
       </c>
       <c r="I20" s="5">
-        <v>32.019001007080078</v>
+        <v>32.281051635742188</v>
       </c>
       <c r="J20" s="5">
-        <v>7.4146504402160645</v>
+        <v>7.491541862487793</v>
       </c>
       <c r="K20" s="5">
-        <v>5.1148538589477539</v>
+        <v>5.1145191192626953</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
@@ -5209,31 +5353,31 @@
         <v>44</v>
       </c>
       <c r="C21" s="5">
-        <v>2.1059925556182861</v>
+        <v>2.1061594486236572</v>
       </c>
       <c r="D21" s="5">
-        <v>0.22971738874912262</v>
+        <v>0.22970578074455261</v>
       </c>
       <c r="E21" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F21" s="5">
-        <v>9.8639764785766602</v>
+        <v>9.9404172897338867</v>
       </c>
       <c r="G21" s="27">
-        <v>1.3506269454956055</v>
+        <v>1.3846265077590942</v>
       </c>
       <c r="H21" s="5">
-        <v>2.0745501518249512</v>
+        <v>2.0754926204681396</v>
       </c>
       <c r="I21" s="5">
-        <v>38.137466430664063</v>
+        <v>38.53094482421875</v>
       </c>
       <c r="J21" s="5">
-        <v>8.4282569885253906</v>
+        <v>8.526580810546875</v>
       </c>
       <c r="K21" s="5">
-        <v>5.3863058090209961</v>
+        <v>5.5517621040344238</v>
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
@@ -5244,31 +5388,31 @@
         <v>45</v>
       </c>
       <c r="C22" s="5">
-        <v>2.70145583152771</v>
+        <v>2.7016963958740234</v>
       </c>
       <c r="D22" s="5">
-        <v>0.38778284192085266</v>
+        <v>0.38776093721389771</v>
       </c>
       <c r="E22" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F22" s="5">
-        <v>11.805631637573242</v>
+        <v>12.022501945495605</v>
       </c>
       <c r="G22" s="27">
-        <v>1.653501033782959</v>
+        <v>1.681121826171875</v>
       </c>
       <c r="H22" s="5">
-        <v>0.53427368402481079</v>
+        <v>0.53459256887435913</v>
       </c>
       <c r="I22" s="5">
-        <v>48.287723541259766</v>
+        <v>48.531871795654297</v>
       </c>
       <c r="J22" s="5">
-        <v>10.039608001708984</v>
+        <v>10.165729522705078</v>
       </c>
       <c r="K22" s="5">
-        <v>5.9522151947021484</v>
+        <v>6.0168004035949707</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
@@ -5279,31 +5423,31 @@
         <v>46</v>
       </c>
       <c r="C23" s="5">
-        <v>3.5990362167358398</v>
+        <v>3.686119556427002</v>
       </c>
       <c r="D23" s="5">
-        <v>0.69693207740783691</v>
+        <v>0.75049841403961182</v>
       </c>
       <c r="E23" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F23" s="5">
-        <v>13.223735809326172</v>
+        <v>13.322453498840332</v>
       </c>
       <c r="G23" s="27">
-        <v>2.0221576690673828</v>
+        <v>2.0465779304504395</v>
       </c>
       <c r="H23" s="5">
-        <v>2.0345284938812256</v>
+        <v>2.0368802547454834</v>
       </c>
       <c r="I23" s="5">
-        <v>55.239879608154297</v>
+        <v>55.687202453613281</v>
       </c>
       <c r="J23" s="5">
-        <v>10.733746528625488</v>
+        <v>10.863153457641602</v>
       </c>
       <c r="K23" s="5">
-        <v>7.3967657089233398</v>
+        <v>7.3968939781188965</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.25">
@@ -5314,31 +5458,31 @@
         <v>47</v>
       </c>
       <c r="C24" s="5">
-        <v>4.0778775215148926</v>
+        <v>4.1232419013977051</v>
       </c>
       <c r="D24" s="5">
-        <v>0.41777944564819336</v>
+        <v>0.41775259375572205</v>
       </c>
       <c r="E24" s="7" t="s">
         <v>11</v>
       </c>
       <c r="F24" s="5">
-        <v>13.898367881774902</v>
+        <v>14.197780609130859</v>
       </c>
       <c r="G24" s="27">
-        <v>1.9988934993743896</v>
+        <v>2.0450842380523682</v>
       </c>
       <c r="H24" s="5">
-        <v>1.4025477170944214</v>
+        <v>1.4877262115478516</v>
       </c>
       <c r="I24" s="5">
-        <v>62.366790771484375</v>
+        <v>63.325370788574219</v>
       </c>
       <c r="J24" s="5">
-        <v>10.95622444152832</v>
+        <v>11.107912063598633</v>
       </c>
       <c r="K24" s="5">
-        <v>6.3790988922119141</v>
+        <v>6.4143924713134766</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.25">
@@ -5349,31 +5493,31 @@
         <v>48</v>
       </c>
       <c r="C25" s="5">
-        <v>3.2319228649139404</v>
+        <v>3.3262591361999512</v>
       </c>
       <c r="D25" s="5">
-        <v>0.4095381498336792</v>
+        <v>0.46069973707199097</v>
       </c>
       <c r="E25" s="5">
         <v>0</v>
       </c>
       <c r="F25" s="5">
-        <v>13.500035285949707</v>
+        <v>13.703057289123535</v>
       </c>
       <c r="G25" s="27">
-        <v>1.9556571245193481</v>
+        <v>1.9836174249649048</v>
       </c>
       <c r="H25" s="5">
-        <v>1.6725915670394897</v>
+        <v>1.6283664703369141</v>
       </c>
       <c r="I25" s="5">
-        <v>61.3614501953125</v>
+        <v>62.060493469238281</v>
       </c>
       <c r="J25" s="5">
-        <v>9.6861410140991211</v>
+        <v>9.8186845779418945</v>
       </c>
       <c r="K25" s="5">
-        <v>5.1365103721618652</v>
+        <v>5.1852922439575195</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.25">
@@ -5384,31 +5528,31 @@
         <v>49</v>
       </c>
       <c r="C26" s="5">
-        <v>2.9435861110687256</v>
+        <v>3.042595386505127</v>
       </c>
       <c r="D26" s="5">
-        <v>0.4037720263004303</v>
+        <v>0.4542144238948822</v>
       </c>
       <c r="E26" s="5">
         <v>0</v>
       </c>
       <c r="F26" s="5">
-        <v>12.031736373901367</v>
+        <v>12.218108177185059</v>
       </c>
       <c r="G26" s="27">
-        <v>2.055109977722168</v>
+        <v>2.0909490585327148</v>
       </c>
       <c r="H26" s="5">
-        <v>0.95193743705749512</v>
+        <v>0.95357799530029297</v>
       </c>
       <c r="I26" s="5">
-        <v>63.576705932617188</v>
+        <v>64.379653930664063</v>
       </c>
       <c r="J26" s="5">
-        <v>9.639404296875</v>
+        <v>9.7886390686035156</v>
       </c>
       <c r="K26" s="5">
-        <v>4.7953572273254395</v>
+        <v>4.8287463188171387</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.25">
@@ -5419,31 +5563,31 @@
         <v>50</v>
       </c>
       <c r="C27" s="6">
-        <v>3.0222606658935547</v>
+        <v>3.1771197319030762</v>
       </c>
       <c r="D27" s="6">
-        <v>0.30021810531616211</v>
+        <v>0.35022801160812378</v>
       </c>
       <c r="E27" s="6">
         <v>0</v>
       </c>
       <c r="F27" s="6">
-        <v>10.208695411682129</v>
+        <v>10.32520580291748</v>
       </c>
       <c r="G27" s="27">
-        <v>1.5673477649688721</v>
+        <v>1.59928297996521</v>
       </c>
       <c r="H27" s="6">
-        <v>0.73566251993179321</v>
+        <v>0.79651123285293579</v>
       </c>
       <c r="I27" s="6">
-        <v>51.927864074707031</v>
+        <v>52.8101806640625</v>
       </c>
       <c r="J27" s="6">
-        <v>7.9456515312194824</v>
+        <v>8.0745458602905273</v>
       </c>
       <c r="K27" s="5">
-        <v>3.2160098552703857</v>
+        <v>3.251598596572876</v>
       </c>
     </row>
     <row r="28" spans="1:11" x14ac:dyDescent="0.25">
@@ -5454,31 +5598,31 @@
         <v>51</v>
       </c>
       <c r="C28" s="6">
-        <v>1.9826321601867676</v>
+        <v>1.9835004806518555</v>
       </c>
       <c r="D28" s="6">
-        <v>0.49713179469108582</v>
+        <v>0.49708780646324158</v>
       </c>
       <c r="E28" s="6">
         <v>0</v>
       </c>
       <c r="F28" s="6">
-        <v>7.4627618789672852</v>
+        <v>7.6170430183410645</v>
       </c>
       <c r="G28" s="28">
-        <v>1.3112838268280029</v>
+        <v>1.3434337377548218</v>
       </c>
       <c r="H28" s="6">
-        <v>0.45405703783035278</v>
+        <v>0.46413716673851013</v>
       </c>
       <c r="I28" s="6">
-        <v>38.002532958984375</v>
+        <v>38.460765838623047</v>
       </c>
       <c r="J28" s="6">
-        <v>5.0520291328430176</v>
+        <v>5.1536784172058105</v>
       </c>
       <c r="K28" s="5">
-        <v>1.6268144845962524</v>
+        <v>1.6722300052642822</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
@@ -5489,31 +5633,31 @@
         <v>52</v>
       </c>
       <c r="C29" s="5">
-        <v>1.4814083576202393</v>
+        <v>1.4821109771728516</v>
       </c>
       <c r="D29" s="5">
-        <v>0.69114881753921509</v>
+        <v>0.74044090509414673</v>
       </c>
       <c r="E29" s="5">
         <v>0</v>
       </c>
       <c r="F29" s="5">
-        <v>7.4834222793579102</v>
+        <v>7.6601696014404297</v>
       </c>
       <c r="G29" s="5">
-        <v>1.6556856632232666</v>
+        <v>1.7128785848617554</v>
       </c>
       <c r="H29" s="5">
-        <v>0.5808570384979248</v>
+        <v>0.58790099620819092</v>
       </c>
       <c r="I29" s="5">
-        <v>36.996898651123047</v>
+        <v>37.600406646728516</v>
       </c>
       <c r="J29" s="5">
-        <v>5.5417447090148926</v>
+        <v>5.6244697570800781</v>
       </c>
       <c r="K29" s="5">
-        <v>1.6963057518005371</v>
+        <v>1.7773818969726563</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
@@ -5524,31 +5668,31 @@
         <v>1</v>
       </c>
       <c r="C30" s="6">
-        <v>2.1214745044708252</v>
+        <v>2.2342774868011475</v>
       </c>
       <c r="D30" s="6">
-        <v>1.0657422542572021</v>
+        <v>1.065638542175293</v>
       </c>
       <c r="E30" s="6">
         <v>0</v>
       </c>
       <c r="F30" s="6">
-        <v>6.1663012504577637</v>
+        <v>6.3414874076843262</v>
       </c>
       <c r="G30" s="6">
-        <v>2.1537556648254395</v>
+        <v>2.2682125568389893</v>
       </c>
       <c r="H30" s="6">
-        <v>0.79365479946136475</v>
+        <v>0.79344689846038818</v>
       </c>
       <c r="I30" s="6">
-        <v>28.81214714050293</v>
+        <v>29.332340240478516</v>
       </c>
       <c r="J30" s="6">
-        <v>5.3684711456298828</v>
+        <v>5.5113825798034668</v>
       </c>
       <c r="K30" s="6">
-        <v>1.5653960704803467</v>
+        <v>1.5924555063247681</v>
       </c>
     </row>
     <row r="31" spans="1:11" x14ac:dyDescent="0.25">
@@ -5559,31 +5703,31 @@
         <v>2</v>
       </c>
       <c r="C31" s="6">
-        <v>2.8614578247070313</v>
+        <v>2.9203550815582275</v>
       </c>
       <c r="D31" s="6">
-        <v>1.2188403606414795</v>
+        <v>1.2674882411956787</v>
       </c>
       <c r="E31" s="6">
-        <v>0.67285466194152832</v>
+        <v>0.67241132259368896</v>
       </c>
       <c r="F31" s="6">
-        <v>4.765934944152832</v>
+        <v>4.9700899124145508</v>
       </c>
       <c r="G31" s="6">
-        <v>2.1429381370544434</v>
+        <v>2.2266185283660889</v>
       </c>
       <c r="H31" s="6">
-        <v>0.86481451988220215</v>
+        <v>0.94868725538253784</v>
       </c>
       <c r="I31" s="6">
-        <v>19.847890853881836</v>
+        <v>20.174749374389648</v>
       </c>
       <c r="J31" s="6">
-        <v>3.9387197494506836</v>
+        <v>4.0606174468994141</v>
       </c>
       <c r="K31" s="6">
-        <v>1.629551887512207</v>
+        <v>1.7148321866989136</v>
       </c>
     </row>
     <row r="32" spans="1:11" x14ac:dyDescent="0.25">
@@ -5594,31 +5738,31 @@
         <v>3</v>
       </c>
       <c r="C32" s="6">
-        <v>2.643326997756958</v>
+        <v>2.7625722885131836</v>
       </c>
       <c r="D32" s="6">
-        <v>1.3464261293411255</v>
+        <v>1.5018576383590698</v>
       </c>
       <c r="E32" s="6">
-        <v>0.21653364598751068</v>
+        <v>0.21626812219619751</v>
       </c>
       <c r="F32" s="6">
-        <v>5.2066221237182617</v>
+        <v>5.5170822143554688</v>
       </c>
       <c r="G32" s="6">
-        <v>2.077000617980957</v>
+        <v>2.2224414348602295</v>
       </c>
       <c r="H32" s="6">
-        <v>0.81767809391021729</v>
+        <v>0.92679446935653687</v>
       </c>
       <c r="I32" s="6">
-        <v>15.927743911743164</v>
+        <v>16.285514831542969</v>
       </c>
       <c r="J32" s="6">
-        <v>4.5957436561584473</v>
+        <v>5.1789765357971191</v>
       </c>
       <c r="K32" s="6">
-        <v>1.9159368276596069</v>
+        <v>2.0401084423065186</v>
       </c>
     </row>
     <row r="33" spans="1:11" x14ac:dyDescent="0.25">
@@ -5629,31 +5773,31 @@
         <v>4</v>
       </c>
       <c r="C33" s="6">
-        <v>3.367321252822876</v>
+        <v>3.6706478595733643</v>
       </c>
       <c r="D33" s="6">
-        <v>0.98522168397903442</v>
+        <v>1.1498841047286987</v>
       </c>
       <c r="E33" s="6">
-        <v>0.61671864986419678</v>
+        <v>0.61545848846435547</v>
       </c>
       <c r="F33" s="6">
-        <v>4.9932241439819336</v>
+        <v>5.4210305213928223</v>
       </c>
       <c r="G33" s="6">
-        <v>1.8075586557388306</v>
+        <v>2.0890429019927979</v>
       </c>
       <c r="H33" s="6">
-        <v>0.64373767375946045</v>
+        <v>0.7637590765953064</v>
       </c>
       <c r="I33" s="6">
-        <v>18.574298858642578</v>
+        <v>20.503454208374023</v>
       </c>
       <c r="J33" s="6">
-        <v>5.109654426574707</v>
+        <v>5.8318877220153809</v>
       </c>
       <c r="K33" s="6">
-        <v>1.6037262678146362</v>
+        <v>1.9167156219482422</v>
       </c>
     </row>
     <row r="34" spans="1:11" x14ac:dyDescent="0.25">
@@ -5664,31 +5808,31 @@
         <v>5</v>
       </c>
       <c r="C34" s="6">
-        <v>3.3671786785125732</v>
+        <v>3.737518310546875</v>
       </c>
       <c r="D34" s="6">
-        <v>0.75598931312561035</v>
+        <v>0.98938566446304321</v>
       </c>
       <c r="E34" s="6">
-        <v>0.23850096762180328</v>
+        <v>0.35687816143035889</v>
       </c>
       <c r="F34" s="6">
-        <v>5.3307600021362305</v>
+        <v>5.805516242980957</v>
       </c>
       <c r="G34" s="6">
-        <v>1.6343907117843628</v>
+        <v>1.8839800357818604</v>
       </c>
       <c r="H34" s="6">
-        <v>0.67584240436553955</v>
+        <v>0.81595903635025024</v>
       </c>
       <c r="I34" s="6">
-        <v>21.443395614624023</v>
+        <v>24.302783966064453</v>
       </c>
       <c r="J34" s="6">
-        <v>6.1963610649108887</v>
+        <v>7.2750115394592285</v>
       </c>
       <c r="K34" s="6">
-        <v>2.045595645904541</v>
+        <v>2.3932876586914063</v>
       </c>
     </row>
     <row r="35" spans="1:11" x14ac:dyDescent="0.25">
@@ -5699,98 +5843,242 @@
         <v>6</v>
       </c>
       <c r="C35" s="6">
-        <v>3.5320274829864502</v>
+        <v>4.0932998657226563</v>
       </c>
       <c r="D35" s="6">
-        <v>1.2890362739562988</v>
+        <v>1.3518719673156738</v>
       </c>
       <c r="E35" s="6">
-        <v>0.40622085332870483</v>
+        <v>0.40517202019691467</v>
       </c>
       <c r="F35" s="6">
-        <v>4.3368673324584961</v>
+        <v>5.2111330032348633</v>
       </c>
       <c r="G35" s="6">
-        <v>1.446558952331543</v>
+        <v>1.9493025541305542</v>
       </c>
       <c r="H35" s="6">
-        <v>0.59168535470962524</v>
+        <v>0.82344377040863037</v>
       </c>
       <c r="I35" s="6">
-        <v>21.700887680053711</v>
+        <v>27.358386993408203</v>
       </c>
       <c r="J35" s="6">
-        <v>5.1318116188049316</v>
+        <v>7.2383108139038086</v>
       </c>
       <c r="K35" s="6">
-        <v>1.7762467861175537</v>
+        <v>2.5349380970001221</v>
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="6"/>
-      <c r="I36" s="6"/>
-      <c r="J36" s="6"/>
-      <c r="K36" s="6"/>
+      <c r="A36" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B36" s="2">
+        <v>7</v>
+      </c>
+      <c r="C36" s="6">
+        <v>1.9396251440048218</v>
+      </c>
+      <c r="D36" s="6">
+        <v>0.76234233379364014</v>
+      </c>
+      <c r="E36" s="6">
+        <v>0.3683987557888031</v>
+      </c>
+      <c r="F36" s="6">
+        <v>4.5480761528015137</v>
+      </c>
+      <c r="G36" s="6">
+        <v>1.5820398330688477</v>
+      </c>
+      <c r="H36" s="6">
+        <v>0.78709602355957031</v>
+      </c>
+      <c r="I36" s="6">
+        <v>25.886768341064453</v>
+      </c>
+      <c r="J36" s="6">
+        <v>6.6495299339294434</v>
+      </c>
+      <c r="K36" s="6">
+        <v>2.801030158996582</v>
+      </c>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C37" s="6"/>
-      <c r="D37" s="6"/>
-      <c r="E37" s="6"/>
-      <c r="F37" s="6"/>
-      <c r="G37" s="6"/>
-      <c r="H37" s="6"/>
-      <c r="I37" s="6"/>
-      <c r="J37" s="6"/>
-      <c r="K37" s="6"/>
+      <c r="A37" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B37" s="2">
+        <v>8</v>
+      </c>
+      <c r="C37" s="6">
+        <v>2.3299543857574463</v>
+      </c>
+      <c r="D37" s="6">
+        <v>0.58268606662750244</v>
+      </c>
+      <c r="E37" s="6">
+        <v>8.6692601442337036E-2</v>
+      </c>
+      <c r="F37" s="6">
+        <v>3.8013887405395508</v>
+      </c>
+      <c r="G37" s="6">
+        <v>1.5181224346160889</v>
+      </c>
+      <c r="H37" s="6">
+        <v>0.84484755992889404</v>
+      </c>
+      <c r="I37" s="6">
+        <v>22.593414306640625</v>
+      </c>
+      <c r="J37" s="6">
+        <v>6.6647090911865234</v>
+      </c>
+      <c r="K37" s="6">
+        <v>2.9476399421691895</v>
+      </c>
     </row>
     <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
-      <c r="H38" s="6"/>
-      <c r="I38" s="6"/>
-      <c r="J38" s="6"/>
-      <c r="K38" s="6"/>
+      <c r="A38" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B38" s="2">
+        <v>9</v>
+      </c>
+      <c r="C38" s="6">
+        <v>2.657804012298584</v>
+      </c>
+      <c r="D38" s="6">
+        <v>0.98090630769729614</v>
+      </c>
+      <c r="E38" s="6">
+        <v>0.41549462080001831</v>
+      </c>
+      <c r="F38" s="6">
+        <v>3.2165038585662842</v>
+      </c>
+      <c r="G38" s="6">
+        <v>1.681193470954895</v>
+      </c>
+      <c r="H38" s="6">
+        <v>0.92393654584884644</v>
+      </c>
+      <c r="I38" s="6">
+        <v>21.088592529296875</v>
+      </c>
+      <c r="J38" s="6">
+        <v>5.752161979675293</v>
+      </c>
+      <c r="K38" s="6">
+        <v>2.8332104682922363</v>
+      </c>
     </row>
     <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C39" s="6"/>
-      <c r="D39" s="6"/>
-      <c r="E39" s="6"/>
-      <c r="F39" s="6"/>
-      <c r="G39" s="6"/>
-      <c r="H39" s="6"/>
-      <c r="I39" s="6"/>
-      <c r="J39" s="6"/>
-      <c r="K39" s="6"/>
+      <c r="A39" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B39" s="2">
+        <v>10</v>
+      </c>
+      <c r="C39" s="6">
+        <v>1.8415106534957886</v>
+      </c>
+      <c r="D39" s="6">
+        <v>0.78921717405319214</v>
+      </c>
+      <c r="E39" s="6">
+        <v>0.40306556224822998</v>
+      </c>
+      <c r="F39" s="6">
+        <v>2.9885284900665283</v>
+      </c>
+      <c r="G39" s="6">
+        <v>1.5680297613143921</v>
+      </c>
+      <c r="H39" s="6">
+        <v>0.78931856155395508</v>
+      </c>
+      <c r="I39" s="6">
+        <v>19.34197998046875</v>
+      </c>
+      <c r="J39" s="6">
+        <v>5.6251239776611328</v>
+      </c>
+      <c r="K39" s="6">
+        <v>2.9597456455230713</v>
+      </c>
     </row>
     <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C40" s="6"/>
-      <c r="D40" s="6"/>
-      <c r="E40" s="6"/>
-      <c r="F40" s="6"/>
-      <c r="G40" s="6"/>
-      <c r="H40" s="6"/>
-      <c r="I40" s="6"/>
-      <c r="J40" s="6"/>
-      <c r="K40" s="6"/>
+      <c r="A40" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B40" s="2">
+        <v>11</v>
+      </c>
+      <c r="C40" s="6">
+        <v>2.4209203720092773</v>
+      </c>
+      <c r="D40" s="6">
+        <v>0.5938524603843689</v>
+      </c>
+      <c r="E40" s="6">
+        <v>0.31556069850921631</v>
+      </c>
+      <c r="F40" s="6">
+        <v>2.9298849105834961</v>
+      </c>
+      <c r="G40" s="6">
+        <v>1.1344213485717773</v>
+      </c>
+      <c r="H40" s="6">
+        <v>0.74979996681213379</v>
+      </c>
+      <c r="I40" s="6">
+        <v>19.664699554443359</v>
+      </c>
+      <c r="J40" s="6">
+        <v>7.1730036735534668</v>
+      </c>
+      <c r="K40" s="6">
+        <v>2.742375373840332</v>
+      </c>
     </row>
     <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
-      <c r="H41" s="6"/>
-      <c r="I41" s="6"/>
-      <c r="J41" s="6"/>
-      <c r="K41" s="6"/>
+      <c r="A41" s="2">
+        <v>2022</v>
+      </c>
+      <c r="B41" s="2">
+        <v>12</v>
+      </c>
+      <c r="C41" s="6">
+        <v>1.4059664011001587</v>
+      </c>
+      <c r="D41" s="6">
+        <v>0.33138808608055115</v>
+      </c>
+      <c r="E41" s="6">
+        <v>0.30981981754302979</v>
+      </c>
+      <c r="F41" s="6">
+        <v>2.3262627124786377</v>
+      </c>
+      <c r="G41" s="6">
+        <v>1.0401909351348877</v>
+      </c>
+      <c r="H41" s="6">
+        <v>0.59026157855987549</v>
+      </c>
+      <c r="I41" s="6">
+        <v>17.685932159423828</v>
+      </c>
+      <c r="J41" s="6">
+        <v>5.3557615280151367</v>
+      </c>
+      <c r="K41" s="6">
+        <v>2.1509358882904053</v>
+      </c>
     </row>
     <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C42" s="6"/>

</xml_diff>